<commit_message>
Add zoom scale data to sheet info output.
</commit_message>
<xml_diff>
--- a/Spreadsheet2Json.Tests/testdata/sheetinformation.xlsx
+++ b/Spreadsheet2Json.Tests/testdata/sheetinformation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\program\C#2022\spreadsheet2json\Spreadsheet2Json.Tests\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0834057F-F120-4984-B9FC-2FA0C23B5630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12CC7FE-FC04-4A80-B6F9-E8E3AD542709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8076" yWindow="1848" windowWidth="20148" windowHeight="12888" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5196" yWindow="1932" windowWidth="21660" windowHeight="14316" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="visible" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="protect_password" sheetId="5" r:id="rId5"/>
     <sheet name="active" sheetId="6" r:id="rId6"/>
     <sheet name="selected" sheetId="7" r:id="rId7"/>
+    <sheet name="zoom150" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>This sheet is visible.</t>
     <phoneticPr fontId="1"/>
@@ -58,6 +59,10 @@
   </si>
   <si>
     <t>This sheet is selected.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Zoom scale 150%</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -530,4 +535,23 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE663E2-F355-49BE-930A-C5DF00553CAF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>